<commit_message>
Addition of absent genes to network.
</commit_message>
<xml_diff>
--- a/Maaike/Network/Genes S. cerevisiae.xlsx
+++ b/Maaike/Network/Genes S. cerevisiae.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAP Mariahoeve\Desktop\BEP\Network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAP Mariahoeve\Desktop\BEP\Git\Maaike\Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF963BE-97C0-4AD4-A846-F8E2753C6B58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBA244E-0694-49FE-AF29-56703AD45D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="75" windowWidth="10695" windowHeight="7875" xr2:uid="{580E24E2-5C06-4C76-9F5F-54DCA5E8B43D}"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="10560" windowHeight="10140" xr2:uid="{580E24E2-5C06-4C76-9F5F-54DCA5E8B43D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="Absent" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
     <t>Axl2</t>
   </si>
@@ -125,65 +126,254 @@
     <t>Rsr1</t>
   </si>
   <si>
+    <t>Sec15</t>
+  </si>
+  <si>
+    <t>Sec3</t>
+  </si>
+  <si>
+    <t>Sec4</t>
+  </si>
+  <si>
+    <t>SepA</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Skm1</t>
+  </si>
+  <si>
+    <t>Spa2</t>
+  </si>
+  <si>
+    <t>Ste20</t>
+  </si>
+  <si>
+    <t>Swi4</t>
+  </si>
+  <si>
+    <t>Tea1</t>
+  </si>
+  <si>
+    <t>Ubi4</t>
+  </si>
+  <si>
+    <t>Ustilago maydis</t>
+  </si>
+  <si>
+    <t>Schizosaccharomyces pombe</t>
+  </si>
+  <si>
+    <t>Ustilago maydis/Neurospora crassa</t>
+  </si>
+  <si>
+    <t>Ustilago maydis, staat wel in SGD</t>
+  </si>
+  <si>
+    <t>YIL140W</t>
+  </si>
+  <si>
+    <t>YBR200W</t>
+  </si>
+  <si>
+    <t>YER155C</t>
+  </si>
+  <si>
+    <t>YPL115C</t>
+  </si>
+  <si>
+    <t>YPL161C</t>
+  </si>
+  <si>
+    <t>YNL271C</t>
+  </si>
+  <si>
+    <t>YBL085W</t>
+  </si>
+  <si>
+    <t>YER114C</t>
+  </si>
+  <si>
+    <t>YCL012W</t>
+  </si>
+  <si>
+    <t>YAL041W</t>
+  </si>
+  <si>
+    <t>YLR229C</t>
+  </si>
+  <si>
+    <t>YNL298W</t>
+  </si>
+  <si>
+    <t>YDR273W</t>
+  </si>
+  <si>
+    <t>YHR061C</t>
+  </si>
+  <si>
+    <t>YDR309C</t>
+  </si>
+  <si>
+    <t>YPL242C</t>
+  </si>
+  <si>
+    <t>YOR188W</t>
+  </si>
+  <si>
+    <t>YGR014W</t>
+  </si>
+  <si>
+    <t>YNL293W</t>
+  </si>
+  <si>
+    <t>YOL112W</t>
+  </si>
+  <si>
+    <t>YDL167C</t>
+  </si>
+  <si>
+    <t>YNL098C</t>
+  </si>
+  <si>
+    <t>YDL135C</t>
+  </si>
+  <si>
+    <t>YOR127W</t>
+  </si>
+  <si>
+    <t>YDR379W</t>
+  </si>
+  <si>
+    <t>YIL118W</t>
+  </si>
+  <si>
+    <t>YGR152C</t>
+  </si>
+  <si>
+    <t>YGL233W</t>
+  </si>
+  <si>
+    <t>YER008C</t>
+  </si>
+  <si>
+    <t>YFL005W</t>
+  </si>
+  <si>
+    <t>YOL113W</t>
+  </si>
+  <si>
+    <t>YLL021W</t>
+  </si>
+  <si>
+    <t>YHL007C</t>
+  </si>
+  <si>
+    <t>YER111C</t>
+  </si>
+  <si>
+    <t>YOR337W</t>
+  </si>
+  <si>
+    <t>YLL039C</t>
+  </si>
+  <si>
+    <t>SCD1</t>
+  </si>
+  <si>
+    <t>U. maydis, staat wel in SGD</t>
+  </si>
+  <si>
+    <t>SPBC16E9.02c</t>
+  </si>
+  <si>
+    <t>S. pombe</t>
+  </si>
+  <si>
+    <t>SPCC895.05.1</t>
+  </si>
+  <si>
+    <t>U. maydis</t>
+  </si>
+  <si>
+    <t>UMAG_00774</t>
+  </si>
+  <si>
     <t>Scd1</t>
   </si>
   <si>
-    <t>Sec15</t>
-  </si>
-  <si>
-    <t>Sec3</t>
-  </si>
-  <si>
-    <t>Sec4</t>
-  </si>
-  <si>
-    <t>SepA</t>
-  </si>
-  <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>Skm1</t>
-  </si>
-  <si>
-    <t>Spa2</t>
-  </si>
-  <si>
-    <t>Ste20</t>
-  </si>
-  <si>
-    <t>Swi4</t>
-  </si>
-  <si>
-    <t>Tea1</t>
-  </si>
-  <si>
-    <t>Ubi4</t>
-  </si>
-  <si>
-    <t>Ustilago maydis</t>
-  </si>
-  <si>
-    <t>Schizosaccharomyces pombe</t>
-  </si>
-  <si>
-    <t>Ustilago maydis/Neurospora crassa</t>
-  </si>
-  <si>
-    <t>Ustilago maydis, staat wel in SGD</t>
-  </si>
-  <si>
-    <t>Ustilago maydis, DIA1/2/3/4 zijn wel vindbaar</t>
+    <t> SPAC16E8.09.1</t>
+  </si>
+  <si>
+    <t>YDR469W</t>
+  </si>
+  <si>
+    <t>U. maydis, N. crassa</t>
+  </si>
+  <si>
+    <t>EFNCRP00000007602</t>
+  </si>
+  <si>
+    <t>UM01141</t>
+  </si>
+  <si>
+    <t>Drf1</t>
+  </si>
+  <si>
+    <t>New method:</t>
+  </si>
+  <si>
+    <t>Amino sequence of gene is found on STRING. The SGD fungi-blast is then used to find the orthologs. These are found in the other tabs.</t>
+  </si>
+  <si>
+    <t>Old methods:</t>
+  </si>
+  <si>
+    <t>Don1 present in S. cerevisiae (https://www.yeastgenome.org/locus/S000002681), contradictory to article</t>
+  </si>
+  <si>
+    <t>For3 "no apparent S. cerevisiae ortholog" (https://www.pombase.org/gene/SPCC895.05). PomBase used, with the orthologs of its interactors</t>
+  </si>
+  <si>
+    <t>Rac1 present U. maydis, interactions from STRING, converted to their S. cerevisiae orthologs in FungiDB</t>
+  </si>
+  <si>
+    <t>Cdc24 in S. cerevisiae is an ortholog of Scd1 in S. pombe (https://www.pombase.org/gene/SPAC16E8.09)</t>
+  </si>
+  <si>
+    <t>SepA present in N. crassa, U. maydis, interactions from STRING, converted to their S. cerevisiae orthologs in FungiDB</t>
+  </si>
+  <si>
+    <t>Dia present U. maydis, interactions from STRING, converted to their S. cerevisiae orthologs in FungiDB</t>
+  </si>
+  <si>
+    <t>CDC24</t>
+  </si>
+  <si>
+    <t>YAL024C</t>
+  </si>
+  <si>
+    <t>YCL014W</t>
+  </si>
+  <si>
+    <t>Komt niet voor is SCMD2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,13 +386,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333330"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,12 +410,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,13 +432,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -561,286 +757,512 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E35BF9-AEC1-4018-888A-A8EA37EC6CA4}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="3"/>
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="3"/>
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797D7D2D-E343-494F-A9D0-9AEA55B96AC5}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3872138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>